<commit_message>
Added book interaction and modified headphone and notebook interaction
</commit_message>
<xml_diff>
--- a/Assets/DesignDocuments/Assets.xlsx
+++ b/Assets/DesignDocuments/Assets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\letis\Projects\UnityProjects\interactive-classroom-experience\Assets\Design Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\letis\Projects\UnityProjects\interactive-classroom-experience\Assets\DesignDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C352E18-C274-459E-9776-9ACD25DE5366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0740A68-9787-4357-B3C5-5B62AB709722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credits" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="120">
   <si>
     <t>Use</t>
   </si>
@@ -305,9 +305,6 @@
     <t>.cs</t>
   </si>
   <si>
-    <t>Opens and closes the notebook UI panel so the player can read the note</t>
-  </si>
-  <si>
     <t>First-person controller for walking, jumping and crouching inside the classroom</t>
   </si>
   <si>
@@ -372,6 +369,27 @@
   </si>
   <si>
     <t>https://youtu.be/UdTzq4pnB6o?si=EutW5CCz8_l58VcB</t>
+  </si>
+  <si>
+    <t>BookInfoInteraction</t>
+  </si>
+  <si>
+    <t>HeadphonesInteraction</t>
+  </si>
+  <si>
+    <t>InteractionHintUI</t>
+  </si>
+  <si>
+    <t>Opens and closes the book UI panel so the player can read the note</t>
+  </si>
+  <si>
+    <t>Plays and pauses music</t>
+  </si>
+  <si>
+    <t>Opens+A8:G10 and closes the notebook UI panel so the player can read the note</t>
+  </si>
+  <si>
+    <t>Gives hint for each interaction</t>
   </si>
 </sst>
 </file>
@@ -772,7 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -821,7 +839,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
@@ -841,7 +859,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
@@ -861,7 +879,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -881,7 +899,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
@@ -901,7 +919,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>23</v>
@@ -921,7 +939,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>26</v>
@@ -941,7 +959,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>28</v>
@@ -961,7 +979,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>30</v>
@@ -981,7 +999,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>32</v>
@@ -1001,7 +1019,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>35</v>
@@ -1021,7 +1039,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>37</v>
@@ -1041,7 +1059,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>39</v>
@@ -1061,7 +1079,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>42</v>
@@ -1081,7 +1099,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>44</v>
@@ -1101,7 +1119,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>47</v>
@@ -1121,7 +1139,7 @@
         <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>51</v>
@@ -1141,7 +1159,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>53</v>
@@ -1161,7 +1179,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>55</v>
@@ -1181,7 +1199,7 @@
         <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E20" t="s">
         <v>71</v>
@@ -1201,7 +1219,7 @@
         <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E21" t="s">
         <v>72</v>
@@ -1221,7 +1239,7 @@
         <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E22" t="s">
         <v>73</v>
@@ -1241,10 +1259,10 @@
         <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F23" t="s">
         <v>75</v>
@@ -1261,10 +1279,10 @@
         <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F24" t="s">
         <v>75</v>
@@ -1281,7 +1299,7 @@
         <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E25" t="s">
         <v>74</v>
@@ -1290,7 +1308,7 @@
         <v>75</v>
       </c>
       <c r="G25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1298,16 +1316,16 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26" t="s">
         <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F26" t="s">
         <v>75</v>
@@ -1343,10 +1361,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6ECF24-1D65-493D-A6A2-E05DB9FC94DC}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="A4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1389,39 +1407,42 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="F2" t="s">
         <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>103</v>
+      </c>
+      <c r="H2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
         <v>61</v>
@@ -1430,18 +1451,18 @@
         <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
         <v>64</v>
@@ -1456,7 +1477,7 @@
         <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="H4" t="s">
         <v>81</v>
@@ -1464,10 +1485,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
         <v>64</v>
@@ -1482,7 +1503,7 @@
         <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H5" t="s">
         <v>81</v>
@@ -1490,10 +1511,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
         <v>64</v>
@@ -1508,7 +1529,7 @@
         <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="H6" t="s">
         <v>81</v>
@@ -1519,7 +1540,7 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
         <v>64</v>
@@ -1534,7 +1555,7 @@
         <v>62</v>
       </c>
       <c r="G7" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="H7" t="s">
         <v>81</v>
@@ -1542,10 +1563,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
         <v>64</v>
@@ -1560,7 +1581,7 @@
         <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="H8" t="s">
         <v>81</v>
@@ -1571,7 +1592,7 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
         <v>64</v>
@@ -1586,7 +1607,7 @@
         <v>62</v>
       </c>
       <c r="G9" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="H9" t="s">
         <v>81</v>
@@ -1594,16 +1615,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="E10" t="s">
         <v>61</v>
@@ -1612,40 +1633,118 @@
         <v>62</v>
       </c>
       <c r="G10" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="H10" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="F11" t="s">
         <v>62</v>
       </c>
       <c r="G11" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="H11" t="s">
-        <v>105</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G4" xr:uid="{8F6ECF24-1D65-493D-A6A2-E05DB9FC94DC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H14">
+    <sortCondition ref="H1:H14"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>